<commit_message>
template change and new jupyter version
</commit_message>
<xml_diff>
--- a/templates/packlista_template_julmaten.xlsx
+++ b/templates/packlista_template_julmaten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\JupyterLab\Kyrkan\WebShopReport\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4B6975-D980-4E87-B12A-450BEF81B7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BB8441-0DD4-4542-BDF2-AF2BC28AF646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Full Name</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Finska</t>
+  </si>
+  <si>
+    <t>Café</t>
   </si>
 </sst>
 </file>
@@ -284,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -385,15 +388,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -452,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1"/>
@@ -466,15 +460,15 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -482,9 +476,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -563,7 +555,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -871,93 +863,93 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.453125" style="33" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="6.1796875" style="33" customWidth="1"/>
-    <col min="4" max="4" width="40.7265625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" style="33" customWidth="1"/>
-    <col min="6" max="6" width="23.26953125" style="33" customWidth="1"/>
-    <col min="7" max="7" width="5.26953125" style="33" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" style="33" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="33" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" style="33" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" style="33" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="31" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="31" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="31" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="31" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="42"/>
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40"/>
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="47" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="35" t="s">
+      <c r="I1" s="46"/>
+      <c r="J1" s="33" t="s">
         <v>4</v>
       </c>
       <c r="K1"/>
     </row>
-    <row r="2" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="50" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="52"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="50"/>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+    <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="39" t="s">
+      <c r="D4" s="55"/>
+      <c r="E4" s="37" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="30" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="15" t="s">
@@ -967,7 +959,7 @@
       <c r="J4" s="8"/>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="4" t="s">
         <v>13</v>
@@ -990,45 +982,45 @@
       <c r="J5"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14">
         <v>1</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="36">
         <v>11</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="53"/>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="31"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="29"/>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" ht="6.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -1041,7 +1033,7 @@
       <c r="J8"/>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="16" t="s">
         <v>21</v>
@@ -1056,7 +1048,7 @@
       <c r="J9" s="18"/>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" ht="21.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="19" t="s">
         <v>22</v>
@@ -1071,11 +1063,13 @@
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="25"/>
+      <c r="I10" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="23"/>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" ht="21.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="19" t="s">
         <v>24</v>
@@ -1093,10 +1087,10 @@
       <c r="I11" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="24"/>
+      <c r="J11" s="23"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" ht="9.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -1125,6 +1119,7 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{a59b6cd5-d141-4a33-8bf1-0ca04484304f}" enabled="1" method="Standard" siteId="{38ae3bcd-9579-4fd4-adda-b42e1495d55a}" contentBits="0" removed="0"/>
   <clbl:label id="{f0785fb4-7cd3-40c0-8122-f25147720244}" enabled="1" method="Standard" siteId="{3619ea90-fa6e-40bf-aa11-2d4a18ad7689}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>